<commit_message>
Updating Modules and Calendar
</commit_message>
<xml_diff>
--- a/resources/Dates_W21A.xlsx
+++ b/resources/Dates_W21A.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
   <si>
     <t>url</t>
   </si>
@@ -222,12 +222,6 @@
   </si>
   <si>
     <t>LogRegAnalysis</t>
-  </si>
-  <si>
-    <t>Logistic -- Summary</t>
-  </si>
-  <si>
-    <t>LogRegSummary</t>
   </si>
 </sst>
 </file>
@@ -611,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,10 +1144,7 @@
         <v>44256</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>